<commit_message>
Modified code for error
</commit_message>
<xml_diff>
--- a/TestData/Login.xlsx
+++ b/TestData/Login.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="ResetPassword" sheetId="3" r:id="rId2"/>
-    <sheet name="Register" sheetId="2" r:id="rId3"/>
+    <sheet name="Shipper Admin" sheetId="4" r:id="rId2"/>
+    <sheet name="ResetPassword" sheetId="3" r:id="rId3"/>
+    <sheet name="Register" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="25">
   <si>
     <t>Automation Test ID</t>
   </si>
@@ -85,13 +86,19 @@
   </si>
   <si>
     <t>Loads_TC004</t>
+  </si>
+  <si>
+    <t>karthikeyan.s@changepond.com</t>
+  </si>
+  <si>
+    <t>Loads_TC005</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +110,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -125,14 +140,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -437,7 +455,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -545,6 +565,80 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -598,7 +692,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>

</xml_diff>